<commit_message>
Ivan MSSQL DB 95% created
</commit_message>
<xml_diff>
--- a/ActivityTracker.xlsx
+++ b/ActivityTracker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iv\Documents\1SHAZIA Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iv\id_web\webshop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>UML Site map</t>
+  </si>
+  <si>
+    <t>MSSQL DB 95% ready</t>
   </si>
 </sst>
 </file>
@@ -181,14 +184,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -507,14 +510,14 @@
   <dimension ref="A2:I78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
     <col min="5" max="5" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39.7109375" style="1" customWidth="1"/>
@@ -543,10 +546,10 @@
       <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="8"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -560,7 +563,7 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="9"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="3"/>
       <c r="I3" s="4" t="s">
         <v>8</v>
@@ -578,7 +581,7 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="9"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="3"/>
       <c r="I4" s="3" t="s">
         <v>6</v>
@@ -596,7 +599,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="9"/>
+      <c r="F5" s="7"/>
       <c r="G5" s="3"/>
       <c r="I5" s="4" t="s">
         <v>8</v>
@@ -614,18 +617,27 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="2">
+        <v>42960</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="9"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -634,7 +646,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="9"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -643,7 +655,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="9"/>
+      <c r="F9" s="7"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -652,7 +664,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="9"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -661,7 +673,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="9"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -670,7 +682,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="9"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -679,7 +691,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="9"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -688,7 +700,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="9"/>
+      <c r="F14" s="7"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -697,7 +709,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="9"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -706,7 +718,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="9"/>
+      <c r="F16" s="7"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -715,7 +727,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="9"/>
+      <c r="F17" s="7"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -724,7 +736,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="9"/>
+      <c r="F18" s="7"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -733,7 +745,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="9"/>
+      <c r="F19" s="7"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -742,7 +754,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="9"/>
+      <c r="F20" s="7"/>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -751,7 +763,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="9"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -760,7 +772,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="9"/>
+      <c r="F22" s="7"/>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -769,7 +781,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="9"/>
+      <c r="F23" s="7"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -778,7 +790,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="9"/>
+      <c r="F24" s="7"/>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -787,7 +799,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="9"/>
+      <c r="F25" s="7"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -796,7 +808,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="9"/>
+      <c r="F26" s="7"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -805,7 +817,7 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="9"/>
+      <c r="F27" s="7"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -814,7 +826,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="9"/>
+      <c r="F28" s="7"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -823,7 +835,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="9"/>
+      <c r="F29" s="7"/>
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -832,7 +844,7 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="9"/>
+      <c r="F30" s="7"/>
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -841,7 +853,7 @@
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="9"/>
+      <c r="F31" s="7"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -850,7 +862,7 @@
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="9"/>
+      <c r="F32" s="7"/>
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -859,7 +871,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="9"/>
+      <c r="F33" s="7"/>
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -868,7 +880,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="9"/>
+      <c r="F34" s="7"/>
       <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -877,7 +889,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="9"/>
+      <c r="F35" s="7"/>
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -886,7 +898,7 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="9"/>
+      <c r="F36" s="7"/>
       <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -895,7 +907,7 @@
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="9"/>
+      <c r="F37" s="7"/>
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -904,7 +916,7 @@
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="9"/>
+      <c r="F38" s="7"/>
       <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -913,7 +925,7 @@
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="9"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -922,7 +934,7 @@
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="9"/>
+      <c r="F40" s="7"/>
       <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -931,7 +943,7 @@
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="9"/>
+      <c r="F41" s="7"/>
       <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -940,7 +952,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="9"/>
+      <c r="F42" s="7"/>
       <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -949,7 +961,7 @@
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="9"/>
+      <c r="F43" s="7"/>
       <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -958,7 +970,7 @@
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="9"/>
+      <c r="F44" s="7"/>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -967,7 +979,7 @@
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="9"/>
+      <c r="F45" s="7"/>
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -976,7 +988,7 @@
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="9"/>
+      <c r="F46" s="7"/>
       <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -985,7 +997,7 @@
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="9"/>
+      <c r="F47" s="7"/>
       <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -994,7 +1006,7 @@
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="9"/>
+      <c r="F48" s="7"/>
       <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1003,7 +1015,7 @@
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="9"/>
+      <c r="F49" s="7"/>
       <c r="G49" s="3"/>
     </row>
     <row r="50" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1012,7 +1024,7 @@
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="9"/>
+      <c r="F50" s="7"/>
       <c r="G50" s="3"/>
     </row>
     <row r="51" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1021,7 +1033,7 @@
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="9"/>
+      <c r="F51" s="7"/>
       <c r="G51" s="3"/>
     </row>
     <row r="52" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1030,7 +1042,7 @@
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="9"/>
+      <c r="F52" s="7"/>
       <c r="G52" s="3"/>
     </row>
     <row r="53" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1039,7 +1051,7 @@
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="9"/>
+      <c r="F53" s="7"/>
       <c r="G53" s="3"/>
     </row>
     <row r="54" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1048,7 +1060,7 @@
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="9"/>
+      <c r="F54" s="7"/>
       <c r="G54" s="3"/>
     </row>
     <row r="55" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1057,7 +1069,7 @@
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
-      <c r="F55" s="9"/>
+      <c r="F55" s="7"/>
       <c r="G55" s="3"/>
     </row>
     <row r="56" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1066,7 +1078,7 @@
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="9"/>
+      <c r="F56" s="7"/>
       <c r="G56" s="3"/>
     </row>
     <row r="57" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1075,7 +1087,7 @@
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
-      <c r="F57" s="9"/>
+      <c r="F57" s="7"/>
       <c r="G57" s="3"/>
     </row>
     <row r="58" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1084,7 +1096,7 @@
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="9"/>
+      <c r="F58" s="7"/>
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1093,7 +1105,7 @@
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="9"/>
+      <c r="F59" s="7"/>
       <c r="G59" s="3"/>
     </row>
     <row r="60" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1102,7 +1114,7 @@
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="9"/>
+      <c r="F60" s="7"/>
       <c r="G60" s="3"/>
     </row>
     <row r="61" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1111,7 +1123,7 @@
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
-      <c r="F61" s="9"/>
+      <c r="F61" s="7"/>
       <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1120,7 +1132,7 @@
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
-      <c r="F62" s="9"/>
+      <c r="F62" s="7"/>
       <c r="G62" s="3"/>
     </row>
     <row r="63" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1129,7 +1141,7 @@
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
-      <c r="F63" s="9"/>
+      <c r="F63" s="7"/>
       <c r="G63" s="3"/>
     </row>
     <row r="64" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1138,7 +1150,7 @@
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="9"/>
+      <c r="F64" s="7"/>
       <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1147,7 +1159,7 @@
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
-      <c r="F65" s="9"/>
+      <c r="F65" s="7"/>
       <c r="G65" s="3"/>
     </row>
     <row r="66" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1156,7 +1168,7 @@
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="9"/>
+      <c r="F66" s="7"/>
       <c r="G66" s="3"/>
     </row>
     <row r="67" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1165,7 +1177,7 @@
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
-      <c r="F67" s="9"/>
+      <c r="F67" s="7"/>
       <c r="G67" s="3"/>
     </row>
     <row r="68" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1174,7 +1186,7 @@
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
-      <c r="F68" s="9"/>
+      <c r="F68" s="7"/>
       <c r="G68" s="3"/>
     </row>
     <row r="69" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1183,7 +1195,7 @@
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
-      <c r="F69" s="9"/>
+      <c r="F69" s="7"/>
       <c r="G69" s="3"/>
     </row>
     <row r="70" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1192,7 +1204,7 @@
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
-      <c r="F70" s="9"/>
+      <c r="F70" s="7"/>
       <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1201,7 +1213,7 @@
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
-      <c r="F71" s="9"/>
+      <c r="F71" s="7"/>
       <c r="G71" s="3"/>
     </row>
     <row r="72" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1210,7 +1222,7 @@
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
-      <c r="F72" s="9"/>
+      <c r="F72" s="7"/>
       <c r="G72" s="3"/>
     </row>
     <row r="73" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1219,7 +1231,7 @@
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
-      <c r="F73" s="9"/>
+      <c r="F73" s="7"/>
       <c r="G73" s="3"/>
     </row>
     <row r="74" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1228,7 +1240,7 @@
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
-      <c r="F74" s="9"/>
+      <c r="F74" s="7"/>
       <c r="G74" s="3"/>
     </row>
     <row r="75" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1237,7 +1249,7 @@
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="9"/>
+      <c r="F75" s="7"/>
       <c r="G75" s="3"/>
     </row>
     <row r="76" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1246,7 +1258,7 @@
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="9"/>
+      <c r="F76" s="7"/>
       <c r="G76" s="3"/>
     </row>
     <row r="77" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1255,7 +1267,7 @@
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="9"/>
+      <c r="F77" s="7"/>
       <c r="G77" s="3"/>
     </row>
     <row r="78" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1264,7 +1276,7 @@
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
-      <c r="F78" s="9"/>
+      <c r="F78" s="7"/>
       <c r="G78" s="3"/>
     </row>
   </sheetData>

</xml_diff>